<commit_message>
updating profile per argonaut discussion
</commit_message>
<xml_diff>
--- a/docs/argo-imaging-diagnosticreport.xlsx
+++ b/docs/argo-imaging-diagnosticreport.xlsx
@@ -571,7 +571,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Encounter], CanonicalType[http://hl7.org/fhir/StructureDefinition/EpisodeOfCare]]}
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter]]}
 </t>
   </si>
   <si>
@@ -815,7 +815,7 @@
 Atomic ValueResultAtomic resultDataTestAnalyteBatteryOrganizer</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/us/core/StructureDefinition/us-core-observationresults]]}
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Observation]]}
 </t>
   </si>
   <si>
@@ -2959,7 +2959,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="17" hidden="true">
+    <row r="17">
       <c r="A17" t="s" s="2">
         <v>173</v>
       </c>
@@ -2975,7 +2975,7 @@
         <v>53</v>
       </c>
       <c r="G17" t="s" s="2">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="H17" t="s" s="2">
         <v>43</v>
@@ -3195,7 +3195,7 @@
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="F19" t="s" s="2">
         <v>53</v>
@@ -4073,7 +4073,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
         <v>250</v>
       </c>
@@ -4089,7 +4089,7 @@
         <v>42</v>
       </c>
       <c r="G27" t="s" s="2">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="H27" t="s" s="2">
         <v>43</v>

</xml_diff>